<commit_message>
fix wrong type Data to Date in excel entity
</commit_message>
<xml_diff>
--- a/rawfile/demo.xlsx
+++ b/rawfile/demo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13">
   <si>
     <t>id</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>是否幸福</t>
+  </si>
+  <si>
+    <t>睡觉时间</t>
   </si>
   <si>
     <t>创建日期</t>
@@ -57,10 +60,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  <numFmts count="7">
+    <numFmt numFmtId="176" formatCode="h:mm:ss;@"/>
+    <numFmt numFmtId="177" formatCode="yyyy/m/d\ h:mm;@"/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="yyyy/m/d;@"/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -100,8 +106,93 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -115,74 +206,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -194,30 +222,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -238,181 +244,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -435,21 +441,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -459,17 +450,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -500,11 +485,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -528,142 +534,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -673,17 +679,20 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1001,23 +1010,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8875" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.8875" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="7"/>
   <cols>
     <col min="2" max="2" width="13.45" customWidth="1"/>
     <col min="3" max="3" width="10.6625" customWidth="1"/>
-    <col min="4" max="4" width="24.6625" customWidth="1"/>
+    <col min="4" max="4" width="24.6625" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.6625" customWidth="1"/>
     <col min="6" max="6" width="12.1125" customWidth="1"/>
-    <col min="7" max="7" width="15.225" customWidth="1"/>
+    <col min="7" max="7" width="15.625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="25.625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1027,7 +1037,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -1036,39 +1046,45 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
+      <c r="B2" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="C2">
         <v>25</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>31508</v>
       </c>
       <c r="E2">
         <v>12345.67</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="3">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.916666666666667</v>
+      </c>
+      <c r="H2" s="3">
         <v>42137.4770833333</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>18</v>
@@ -1076,21 +1092,21 @@
       <c r="F4" t="b">
         <v>1</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <v>42219.6020833333</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>100</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>32874</v>
       </c>
       <c r="E5">
@@ -1099,7 +1115,10 @@
       <c r="F5" t="b">
         <v>0</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
+        <v>0.895833333333333</v>
+      </c>
+      <c r="H5" s="3">
         <v>31520.2229166667</v>
       </c>
     </row>
@@ -1122,7 +1141,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>